<commit_message>
Added EB automation to selendroid
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_Application_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_Application_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="97">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -246,28 +246,6 @@
   </si>
   <si>
     <t>Security token not passed</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(Application_test_link);
-validate2;
-SelectTestToRun(VT200_0004_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-validate4;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(Application_test_link);
-validate2;
-SelectTestToRun(VT200_0005_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-validate4;</t>
   </si>
   <si>
     <t>validate1
@@ -668,7 +646,31 @@
   </si>
   <si>
     <t>wait(3);
-SetStartPage(http://10.233.85.82:9104/app/);</t>
+validate1;
+link_Click(Application_test_link);
+validate2;
+SelectTestToRun(VT200_0004_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ScrollPage(runtest_bottom_xpath);
+ClickRunTest(runtest_bottom_xpath);
+validate4;</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(Application_test_link);
+validate2;
+SelectTestToRun(VT200_0005_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ScrollPage(runtest_bottom_xpath);
+ClickRunTest(runtest_bottom_xpath);
+validate4;</t>
+  </si>
+  <si>
+    <t>wait(3);
+SetStartPage(http://127.0.0.1:8082/app/);</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1154,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J2" sqref="J2:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1213,7 +1215,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -1235,9 +1237,7 @@
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="C3" s="4"/>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1248,10 +1248,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1275,10 +1275,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1302,10 +1302,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1329,10 +1329,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1350,16 +1350,16 @@
         <v>10</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1377,16 +1377,16 @@
         <v>10</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1404,16 +1404,16 @@
         <v>10</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1431,16 +1431,16 @@
         <v>10</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="11" t="s">
         <v>85</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>87</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1464,10 +1464,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1491,10 +1491,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1516,10 +1516,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>

</xml_diff>

<commit_message>
Modified DSL for EB
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_Application_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_Application_JS.xlsx
@@ -301,24 +301,6 @@
 validate4;</t>
   </si>
   <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Application JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0006
-};
-validate4
-{
-validate_Result=/data/data/com.rhomobile.compliancetest_js/rhodata/db/syncdblocal.sqlite
-};</t>
-  </si>
-  <si>
     <t xml:space="preserve">validate1
 {
 validate_PageTitle=Compliance JS specs
@@ -557,24 +539,6 @@
 validate1;
 link_Click(Application_test_link);
 validate2;
-SelectTestToRun(VT200_0011_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-press_Key(home);
-validate4;
-Lock_UnlockScreen(lock);
-Lock_UnlockScreen(unlock);
-launch_App_Device(com.rhomobile.compliancetest_js/com.rhomobile.rhodes.RhodesActivity);
-link_Click(stopCallback_name_xpath);
-validate5;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(Application_test_link);
-validate2;
 SelectTestToRun(VT200_0009_string);
 ClickRunTest(runtest_top_xpath);
 validate3;
@@ -671,6 +635,42 @@
   <si>
     <t>wait(3);
 SetStartPage(http://127.0.0.1:8082/app/);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Application JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0006
+};
+validate4
+{
+validate_Result=/data/data/com.symbol.enterprisebrowser/rhodata/db/syncdblocal.sqlite
+};</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(Application_test_link);
+validate2;
+SelectTestToRun(VT200_0011_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+press_Key(home);
+validate4;
+Lock_UnlockScreen(lock);
+Lock_UnlockScreen(unlock);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+link_Click(stopCallback_name_xpath);
+validate5;</t>
   </si>
 </sst>
 </file>
@@ -1154,7 +1154,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J12"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1215,13 +1215,13 @@
         <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="2" t="s">
@@ -1248,7 +1248,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>70</v>
@@ -1275,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>69</v>
@@ -1305,7 +1305,7 @@
         <v>73</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1329,10 +1329,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1356,10 +1356,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>78</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1383,10 +1383,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1404,16 +1404,16 @@
         <v>10</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1431,16 +1431,16 @@
         <v>10</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1464,10 +1464,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1491,10 +1491,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1516,10 +1516,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>

</xml_diff>

<commit_message>
Added new way to change Config
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_Application_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_Application_JS.xlsx
@@ -633,10 +633,6 @@
 validate4;</t>
   </si>
   <si>
-    <t>wait(3);
-SetStartPage(http://127.0.0.1:8082/app/);</t>
-  </si>
-  <si>
     <t>validate1
 {
 validate_PageTitle=Compliance JS specs
@@ -671,6 +667,18 @@
 launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
 link_Click(stopCallback_name_xpath);
 validate5;</t>
+  </si>
+  <si>
+    <t>wait(3);
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;);
+ChangeConfigxml(Configuration/WebServer,Enabled,&lt;Enabled VALUE="1"/&gt;);
+ChangeConfigxml(Configuration/WebServer,Port,&lt;Port VALUE="8082"/&gt;);
+ChangeConfigxml(Configuration/WebServer,WebFolder,&lt;WebFolder VALUE="\\auto\\ComplianceTest_JS\"/&gt;);
+ChangeConfigxml(Configuration/WebServer,Public,&lt;Public VALUE="1"/&gt;);
+ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="0"/&gt;);
+PushConfigxml;</t>
   </si>
 </sst>
 </file>
@@ -1153,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1163,7 +1171,7 @@
     <col min="2" max="2" width="8.28515625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="74" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="37.140625" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -1201,7 +1209,7 @@
       </c>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="43.5" thickBot="1">
+    <row r="2" spans="1:11" ht="153.75" thickBot="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1221,7 +1229,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="2" t="s">
@@ -1305,7 +1313,7 @@
         <v>73</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1410,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
Added changes config update
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_Application_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_Application_JS.xlsx
@@ -672,11 +672,7 @@
     <t>wait(3);
 PullConfigxml;
 ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
-ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;);
-ChangeConfigxml(Configuration/WebServer,Enabled,&lt;Enabled VALUE="1"/&gt;);
-ChangeConfigxml(Configuration/WebServer,Port,&lt;Port VALUE="8082"/&gt;);
-ChangeConfigxml(Configuration/WebServer,WebFolder,&lt;WebFolder VALUE="\\auto\\ComplianceTest_JS\"/&gt;);
-ChangeConfigxml(Configuration/WebServer,Public,&lt;Public VALUE="1"/&gt;);
+ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;endl  &lt;Enabled VALUE="1"/&gt;endl  &lt;Port VALUE="8082"/&gt;endl  &lt;WebFolder VALUE="\\auto\\ComplianceTest_JS\"/&gt;endl  &lt;Public VALUE="1"/&gt;endl&lt;/WebServer&gt;endl);
 ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="0"/&gt;);
 PushConfigxml;</t>
   </si>
@@ -1162,7 +1158,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1209,7 +1205,7 @@
       </c>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="153.75" thickBot="1">
+    <row r="2" spans="1:11" ht="128.25" thickBot="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Modified javacode for nexus
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_Application_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EB_Application_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="97">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -1157,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1512,7 +1512,9 @@
         <v>1</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E13" s="12" t="s">
         <v>51</v>
       </c>

</xml_diff>